<commit_message>
Moved the delte phase to before the conversion phase to make sure they don't tread on each other's toes
</commit_message>
<xml_diff>
--- a/sample-data/first-fleet-maps.xlsx
+++ b/sample-data/first-fleet-maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="600" windowWidth="25740" windowHeight="14640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24880" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="First Fleet Maps" sheetId="1" r:id="rId1"/>
@@ -514,9 +514,6 @@
     <t>nsw.gov.au/_zoomify/2010/D05895/a1528993.html</t>
   </si>
   <si>
-    <t>Image</t>
-  </si>
-  <si>
     <t>Omeka Type</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>Person</t>
+  </si>
+  <si>
+    <t>Still Image</t>
   </si>
 </sst>
 </file>
@@ -960,7 +960,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -975,7 +975,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>902810</v>
@@ -1028,7 +1028,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F2">
         <v>903932</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>480022</v>
@@ -1069,7 +1069,7 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3">
         <v>862353</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B4">
         <v>480023</v>
@@ -1110,7 +1110,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F4">
         <v>862353</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B5">
         <v>480024</v>
@@ -1151,7 +1151,7 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F5">
         <v>862353</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B6">
         <v>480025</v>
@@ -1192,7 +1192,7 @@
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6">
         <v>862353</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B7">
         <v>480026</v>
@@ -1233,7 +1233,7 @@
         <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7">
         <v>862353</v>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B8">
         <v>480027</v>
@@ -1274,7 +1274,7 @@
         <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F8">
         <v>862353</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B9">
         <v>480028</v>
@@ -1315,7 +1315,7 @@
         <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F9">
         <v>862353</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>480029</v>
@@ -1356,7 +1356,7 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F10">
         <v>862353</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B11">
         <v>480030</v>
@@ -1397,7 +1397,7 @@
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11">
         <v>862353</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B12">
         <v>480031</v>
@@ -1438,7 +1438,7 @@
         <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F12">
         <v>862353</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B13">
         <v>480032</v>
@@ -1479,7 +1479,7 @@
         <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F13">
         <v>862353</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B14">
         <v>480033</v>
@@ -1520,7 +1520,7 @@
         <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F14">
         <v>862353</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B15">
         <v>480034</v>
@@ -1561,7 +1561,7 @@
         <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F15">
         <v>862353</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B16">
         <v>887137</v>
@@ -1602,7 +1602,7 @@
         <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F16">
         <v>889870</v>
@@ -1631,7 +1631,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B17">
         <v>887141</v>
@@ -1643,7 +1643,7 @@
         <v>99</v>
       </c>
       <c r="E17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F17">
         <v>889972</v>
@@ -1672,7 +1672,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B18">
         <v>902815</v>
@@ -1684,7 +1684,7 @@
         <v>106</v>
       </c>
       <c r="E18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F18">
         <v>903940</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B19">
         <v>903891</v>
@@ -1725,7 +1725,7 @@
         <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F19">
         <v>913701</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B20">
         <v>903892</v>
@@ -1766,7 +1766,7 @@
         <v>123</v>
       </c>
       <c r="E20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20">
         <v>913700</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B21">
         <v>903896</v>
@@ -1807,7 +1807,7 @@
         <v>131</v>
       </c>
       <c r="E21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F21">
         <v>913724</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B22">
         <v>909019</v>
@@ -1848,7 +1848,7 @@
         <v>138</v>
       </c>
       <c r="E22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F22">
         <v>910700</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B23">
         <v>478053</v>
@@ -1889,7 +1889,7 @@
         <v>147</v>
       </c>
       <c r="E23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F23">
         <v>861495</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B24">
         <v>902821</v>
@@ -1930,7 +1930,7 @@
         <v>156</v>
       </c>
       <c r="E24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F24">
         <v>903944</v>
@@ -1984,7 +1984,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1993,18 +1993,18 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" t="s">
         <v>170</v>
-      </c>
-      <c r="E1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2032,10 +2032,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
         <v>148</v>
@@ -2043,10 +2043,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
         <v>157</v>

</xml_diff>